<commit_message>
fixed left margin changed data to not have empty row
</commit_message>
<xml_diff>
--- a/components/bower_components/unitedstatesdata.xlsx
+++ b/components/bower_components/unitedstatesdata.xlsx
@@ -956,13 +956,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q233"/>
+  <dimension ref="A1:Q232"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="HV219" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="A232" sqref="A232:XFD232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12100,7 +12100,6 @@
       <c r="P232" s="5"/>
       <c r="Q232" s="5"/>
     </row>
-    <row r="233" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>